<commit_message>
Task 20 Task 21  Task 22 Task 23
</commit_message>
<xml_diff>
--- a/SourceCode/2024/Basics-April2024/Radha/Task 20/Raw Data.xlsx
+++ b/SourceCode/2024/Basics-April2024/Radha/Task 20/Raw Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\RPA\RPA-Developer-in-30-Days\SourceCode\2024\Basics-April2024\Radha\Task 20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B5D8C0-2371-4127-B186-8467F54179F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1388C516-36E7-49DF-8605-156A1E599195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="3570" yWindow="2265" windowWidth="15375" windowHeight="7875" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,24 +26,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <x:si>
     <x:t>lower case</x:t>
   </x:si>
   <x:si>
-    <x:t>Upper Case</x:t>
+    <x:t>upper case</x:t>
   </x:si>
   <x:si>
     <x:t>mno</x:t>
   </x:si>
   <x:si>
+    <x:t>MNO</x:t>
+  </x:si>
+  <x:si>
     <x:t>xyz</x:t>
   </x:si>
   <x:si>
+    <x:t>XYZ</x:t>
+  </x:si>
+  <x:si>
     <x:t>wsg</x:t>
   </x:si>
   <x:si>
+    <x:t>WSG</x:t>
+  </x:si>
+  <x:si>
     <x:t>lpo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LPO</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -376,7 +388,7 @@
   <x:dimension ref="A1:B6"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="B2" sqref="B2"/>
+      <x:selection activeCell="H7" sqref="H7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,7 +396,7 @@
     <x:col min="1" max="1" width="11" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -392,29 +404,44 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <x:c r="B2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A4" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A5" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A6" s="0" t="s">
         <x:v>2</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>3</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>